<commit_message>
Faculty List updation continues
Faculty List updation continues
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/FacultyDetails/FacultyList.xlsx
+++ b/Offline/BusinessManagement/Ops/FacultyDetails/FacultyList.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\FacultyDetails\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6666F0-42C9-479C-BAED-AB205DF3ED96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904B0DFA-9BA5-4EA2-BE0E-357F797FE90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Faculty" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>SlNo</t>
   </si>
@@ -95,6 +95,30 @@
   </si>
   <si>
     <t>93398 18158</t>
+  </si>
+  <si>
+    <t>Sayan Basak</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>Bank Name</t>
+  </si>
+  <si>
+    <t>Bank A/C No</t>
+  </si>
+  <si>
+    <t>IFSC Code</t>
+  </si>
+  <si>
+    <t>Bank Of India</t>
+  </si>
+  <si>
+    <t>402910110001569</t>
+  </si>
+  <si>
+    <t>BKID0004029</t>
   </si>
 </sst>
 </file>
@@ -147,7 +171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -159,6 +183,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -440,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,9 +480,12 @@
     <col min="4" max="4" width="27.21875" customWidth="1"/>
     <col min="5" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -475,8 +504,17 @@
       <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -496,7 +534,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -513,7 +551,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -530,7 +568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -545,6 +583,29 @@
       </c>
       <c r="F5" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>